<commit_message>
update for second draft of weigo report
</commit_message>
<xml_diff>
--- a/Tables/characteristics_switchers.xlsx
+++ b/Tables/characteristics_switchers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Statistics\P27\IMSS\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE3BA5F-42F0-4BED-98C7-9D8EAFA59295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC64C87A-92BB-4BEE-AFC0-8027781C7649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8190" windowWidth="29040" windowHeight="15720" xr2:uid="{31CCF630-13B6-465C-881E-27A289AA3316}"/>
+    <workbookView xWindow="28680" yWindow="-6990" windowWidth="29040" windowHeight="15720" xr2:uid="{31CCF630-13B6-465C-881E-27A289AA3316}"/>
   </bookViews>
   <sheets>
     <sheet name="characteristics_switchers" sheetId="1" r:id="rId1"/>
@@ -184,9 +184,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,6 +193,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -257,25 +257,25 @@
             <v>-0.012***</v>
           </cell>
           <cell r="C5" t="str">
-            <v>-0.011***</v>
+            <v>-0.012***</v>
           </cell>
           <cell r="D5" t="str">
-            <v>-0.0081***</v>
+            <v>-0.0088***</v>
           </cell>
           <cell r="E5" t="str">
-            <v>-0.0076***</v>
+            <v>-0.0078***</v>
           </cell>
           <cell r="F5" t="str">
-            <v>-0.015***</v>
+            <v>-0.016***</v>
           </cell>
           <cell r="G5" t="str">
             <v>-0.015***</v>
           </cell>
           <cell r="H5" t="str">
-            <v>-0.0076***</v>
+            <v>-0.0093***</v>
           </cell>
           <cell r="I5" t="str">
-            <v>-0.0069***</v>
+            <v>-0.0086***</v>
           </cell>
         </row>
         <row r="6">
@@ -286,13 +286,13 @@
             <v>(0.000016)</v>
           </cell>
           <cell r="C6" t="str">
-            <v>(0.000016)</v>
+            <v>(0.000017)</v>
           </cell>
           <cell r="D6" t="str">
-            <v>(0.000013)</v>
+            <v>(0.000014)</v>
           </cell>
           <cell r="E6" t="str">
-            <v>(0.000013)</v>
+            <v>(0.000014)</v>
           </cell>
           <cell r="F6" t="str">
             <v>(0.000016)</v>
@@ -301,7 +301,7 @@
             <v>(0.000016)</v>
           </cell>
           <cell r="H6" t="str">
-            <v>(0.000014)</v>
+            <v>(0.000013)</v>
           </cell>
           <cell r="I6" t="str">
             <v>(0.000014)</v>
@@ -309,28 +309,28 @@
         </row>
         <row r="8">
           <cell r="B8" t="str">
-            <v>0.013***</v>
+            <v>0.015***</v>
           </cell>
           <cell r="C8" t="str">
-            <v>0.010***</v>
+            <v>0.012***</v>
           </cell>
           <cell r="D8" t="str">
-            <v>-0.0099***</v>
+            <v>-0.014***</v>
           </cell>
           <cell r="E8" t="str">
-            <v>-0.013***</v>
+            <v>-0.019***</v>
           </cell>
           <cell r="F8" t="str">
-            <v>0.020***</v>
+            <v>0.021***</v>
           </cell>
           <cell r="G8" t="str">
-            <v>0.018***</v>
+            <v>0.019***</v>
           </cell>
           <cell r="H8" t="str">
-            <v>-0.018***</v>
+            <v>-0.0069***</v>
           </cell>
           <cell r="I8" t="str">
-            <v>-0.022***</v>
+            <v>-0.011***</v>
           </cell>
         </row>
         <row r="9">
@@ -338,22 +338,22 @@
             <v/>
           </cell>
           <cell r="B9" t="str">
-            <v>(0.000020)</v>
+            <v>(0.000021)</v>
           </cell>
           <cell r="C9" t="str">
-            <v>(0.000020)</v>
+            <v>(0.000022)</v>
           </cell>
           <cell r="D9" t="str">
-            <v>(0.000015)</v>
+            <v>(0.000017)</v>
           </cell>
           <cell r="E9" t="str">
-            <v>(0.000016)</v>
+            <v>(0.000018)</v>
           </cell>
           <cell r="F9" t="str">
-            <v>(0.000019)</v>
+            <v>(0.000021)</v>
           </cell>
           <cell r="G9" t="str">
-            <v>(0.000020)</v>
+            <v>(0.000021)</v>
           </cell>
           <cell r="H9" t="str">
             <v>(0.000016)</v>
@@ -370,22 +370,22 @@
             <v>0.014***</v>
           </cell>
           <cell r="D11" t="str">
-            <v>0.0071***</v>
+            <v>0.010***</v>
           </cell>
           <cell r="E11" t="str">
-            <v>0.0038***</v>
+            <v>0.0060***</v>
           </cell>
           <cell r="F11" t="str">
             <v>0.011***</v>
           </cell>
           <cell r="G11" t="str">
-            <v>0.0086***</v>
+            <v>0.0087***</v>
           </cell>
           <cell r="H11" t="str">
-            <v>0.0099***</v>
+            <v>0.0073***</v>
           </cell>
           <cell r="I11" t="str">
-            <v>0.0058***</v>
+            <v>0.0041***</v>
           </cell>
         </row>
         <row r="12">
@@ -399,10 +399,10 @@
             <v>(0.000012)</v>
           </cell>
           <cell r="D12" t="str">
-            <v>(0.0000086)</v>
+            <v>(0.0000087)</v>
           </cell>
           <cell r="E12" t="str">
-            <v>(0.0000091)</v>
+            <v>(0.0000092)</v>
           </cell>
           <cell r="F12" t="str">
             <v>(0.000011)</v>
@@ -411,7 +411,7 @@
             <v>(0.000012)</v>
           </cell>
           <cell r="H12" t="str">
-            <v>(0.0000087)</v>
+            <v>(0.0000086)</v>
           </cell>
           <cell r="I12" t="str">
             <v>(0.0000091)</v>
@@ -419,28 +419,28 @@
         </row>
         <row r="14">
           <cell r="B14" t="str">
-            <v>0.0068***</v>
+            <v>0.0067***</v>
           </cell>
           <cell r="C14" t="str">
-            <v>0.0068***</v>
+            <v>0.0065***</v>
           </cell>
           <cell r="D14" t="str">
-            <v>0.0079***</v>
+            <v>0.0040***</v>
           </cell>
           <cell r="E14" t="str">
+            <v>0.0035***</v>
+          </cell>
+          <cell r="F14" t="str">
+            <v>0.012***</v>
+          </cell>
+          <cell r="G14" t="str">
+            <v>0.012***</v>
+          </cell>
+          <cell r="H14" t="str">
             <v>0.0076***</v>
           </cell>
-          <cell r="F14" t="str">
-            <v>0.013***</v>
-          </cell>
-          <cell r="G14" t="str">
-            <v>0.013***</v>
-          </cell>
-          <cell r="H14" t="str">
-            <v>0.0039***</v>
-          </cell>
           <cell r="I14" t="str">
-            <v>0.0036***</v>
+            <v>0.0072***</v>
           </cell>
         </row>
         <row r="15">
@@ -448,54 +448,54 @@
             <v/>
           </cell>
           <cell r="B15" t="str">
+            <v>(0.0000085)</v>
+          </cell>
+          <cell r="C15" t="str">
             <v>(0.0000086)</v>
           </cell>
-          <cell r="C15" t="str">
-            <v>(0.0000087)</v>
-          </cell>
           <cell r="D15" t="str">
+            <v>(0.0000071)</v>
+          </cell>
+          <cell r="E15" t="str">
+            <v>(0.0000071)</v>
+          </cell>
+          <cell r="F15" t="str">
+            <v>(0.0000082)</v>
+          </cell>
+          <cell r="G15" t="str">
+            <v>(0.0000083)</v>
+          </cell>
+          <cell r="H15" t="str">
             <v>(0.0000066)</v>
           </cell>
-          <cell r="E15" t="str">
+          <cell r="I15" t="str">
             <v>(0.0000067)</v>
-          </cell>
-          <cell r="F15" t="str">
-            <v>(0.0000083)</v>
-          </cell>
-          <cell r="G15" t="str">
-            <v>(0.0000084)</v>
-          </cell>
-          <cell r="H15" t="str">
-            <v>(0.0000072)</v>
-          </cell>
-          <cell r="I15" t="str">
-            <v>(0.0000072)</v>
           </cell>
         </row>
         <row r="17">
           <cell r="B17" t="str">
-            <v>-0.0036***</v>
+            <v>0.0035***</v>
           </cell>
           <cell r="C17" t="str">
-            <v>-0.0042***</v>
+            <v>0.0034***</v>
           </cell>
           <cell r="D17" t="str">
-            <v>-0.00036***</v>
+            <v>0.0013***</v>
           </cell>
           <cell r="E17" t="str">
-            <v>-0.00058***</v>
+            <v>0.0013***</v>
           </cell>
           <cell r="F17" t="str">
-            <v>-0.00045***</v>
+            <v>-0.0024***</v>
           </cell>
           <cell r="G17" t="str">
-            <v>-0.00079***</v>
+            <v>-0.0024***</v>
           </cell>
           <cell r="H17" t="str">
-            <v>-0.0011***</v>
+            <v>-0.00060***</v>
           </cell>
           <cell r="I17" t="str">
-            <v>-0.0016***</v>
+            <v>-0.00065***</v>
           </cell>
         </row>
         <row r="18">
@@ -503,28 +503,28 @@
             <v/>
           </cell>
           <cell r="B18" t="str">
-            <v>(0.0000050)</v>
+            <v>(0.0000043)</v>
           </cell>
           <cell r="C18" t="str">
-            <v>(0.0000052)</v>
+            <v>(0.0000043)</v>
           </cell>
           <cell r="D18" t="str">
-            <v>(0.0000040)</v>
+            <v>(0.0000035)</v>
           </cell>
           <cell r="E18" t="str">
-            <v>(0.0000041)</v>
+            <v>(0.0000035)</v>
           </cell>
           <cell r="F18" t="str">
-            <v>(0.0000049)</v>
+            <v>(0.0000042)</v>
           </cell>
           <cell r="G18" t="str">
-            <v>(0.0000050)</v>
+            <v>(0.0000042)</v>
           </cell>
           <cell r="H18" t="str">
-            <v>(0.0000042)</v>
+            <v>(0.0000035)</v>
           </cell>
           <cell r="I18" t="str">
-            <v>(0.0000043)</v>
+            <v>(0.0000035)</v>
           </cell>
         </row>
         <row r="20">
@@ -532,25 +532,25 @@
             <v>-0.0040***</v>
           </cell>
           <cell r="C20" t="str">
-            <v>0.00035***</v>
+            <v>-0.000030</v>
           </cell>
           <cell r="D20" t="str">
-            <v>-0.00045***</v>
+            <v>-0.0060***</v>
           </cell>
           <cell r="E20" t="str">
-            <v>0.0039***</v>
+            <v>-0.0010***</v>
           </cell>
           <cell r="F20" t="str">
-            <v>0.000057**</v>
+            <v>-0.00041***</v>
           </cell>
           <cell r="G20" t="str">
-            <v>0.0034***</v>
+            <v>0.0028***</v>
           </cell>
           <cell r="H20" t="str">
-            <v>-0.0063***</v>
+            <v>-0.00040***</v>
           </cell>
           <cell r="I20" t="str">
-            <v>-0.0011***</v>
+            <v>0.0037***</v>
           </cell>
         </row>
         <row r="21">
@@ -564,7 +564,7 @@
             <v>(0.000027)</v>
           </cell>
           <cell r="D21" t="str">
-            <v>(0.000021)</v>
+            <v>(0.000020)</v>
           </cell>
           <cell r="E21" t="str">
             <v>(0.000021)</v>
@@ -576,7 +576,7 @@
             <v>(0.000027)</v>
           </cell>
           <cell r="H21" t="str">
-            <v>(0.000020)</v>
+            <v>(0.000021)</v>
           </cell>
           <cell r="I21" t="str">
             <v>(0.000021)</v>
@@ -584,28 +584,28 @@
         </row>
         <row r="23">
           <cell r="B23" t="str">
-            <v>0.00026***</v>
+            <v>-0.0043***</v>
           </cell>
           <cell r="C23" t="str">
-            <v>-0.00022***</v>
+            <v>-0.0032***</v>
           </cell>
           <cell r="D23" t="str">
-            <v>0.0010***</v>
+            <v>-0.0069***</v>
           </cell>
           <cell r="E23" t="str">
-            <v>0.00086***</v>
+            <v>-0.0054***</v>
           </cell>
           <cell r="F23" t="str">
-            <v>0.0013***</v>
+            <v>-0.0033***</v>
           </cell>
           <cell r="G23" t="str">
-            <v>0.0011***</v>
+            <v>-0.0026***</v>
           </cell>
           <cell r="H23" t="str">
-            <v>0.00068***</v>
+            <v>-0.0062***</v>
           </cell>
           <cell r="I23" t="str">
-            <v>0.00033***</v>
+            <v>-0.0049***</v>
           </cell>
         </row>
         <row r="24">
@@ -613,138 +613,109 @@
             <v/>
           </cell>
           <cell r="B24" t="str">
-            <v>(0.000017)</v>
+            <v>(0.000016)</v>
           </cell>
           <cell r="C24" t="str">
-            <v>(0.000018)</v>
+            <v>(0.000016)</v>
           </cell>
           <cell r="D24" t="str">
-            <v>(0.000014)</v>
+            <v>(0.000013)</v>
           </cell>
           <cell r="E24" t="str">
-            <v>(0.000014)</v>
+            <v>(0.000013)</v>
           </cell>
           <cell r="F24" t="str">
-            <v>(0.000017)</v>
+            <v>(0.000016)</v>
           </cell>
           <cell r="G24" t="str">
-            <v>(0.000018)</v>
+            <v>(0.000016)</v>
           </cell>
           <cell r="H24" t="str">
-            <v>(0.000014)</v>
+            <v>(0.000013)</v>
           </cell>
           <cell r="I24" t="str">
-            <v>(0.000015)</v>
+            <v>(0.000013)</v>
           </cell>
         </row>
         <row r="26">
           <cell r="B26" t="str">
-            <v>1298450070</v>
+            <v>0.00022***</v>
           </cell>
           <cell r="C26" t="str">
-            <v>1298450070</v>
+            <v>-0.00023***</v>
           </cell>
           <cell r="D26" t="str">
-            <v>1287678797</v>
+            <v>0.00069***</v>
           </cell>
           <cell r="E26" t="str">
-            <v>1287678797</v>
+            <v>0.00034***</v>
           </cell>
           <cell r="F26" t="str">
-            <v>1298450070</v>
+            <v>0.0013***</v>
           </cell>
           <cell r="G26" t="str">
-            <v>1298450070</v>
+            <v>0.0011***</v>
           </cell>
           <cell r="H26" t="str">
-            <v>1287678797</v>
+            <v>0.0010***</v>
           </cell>
           <cell r="I26" t="str">
-            <v>1287678797</v>
+            <v>0.00088***</v>
           </cell>
         </row>
         <row r="27">
           <cell r="A27" t="str">
-            <v>R-sq</v>
+            <v/>
           </cell>
           <cell r="B27" t="str">
-            <v>0.009</v>
+            <v>(0.000017)</v>
           </cell>
           <cell r="C27" t="str">
-            <v>0.013</v>
+            <v>(0.000018)</v>
           </cell>
           <cell r="D27" t="str">
-            <v>0.012</v>
+            <v>(0.000014)</v>
           </cell>
           <cell r="E27" t="str">
-            <v>0.016</v>
+            <v>(0.000015)</v>
           </cell>
           <cell r="F27" t="str">
-            <v>0.008</v>
+            <v>(0.000017)</v>
           </cell>
           <cell r="G27" t="str">
-            <v>0.011</v>
+            <v>(0.000018)</v>
           </cell>
           <cell r="H27" t="str">
-            <v>0.009</v>
+            <v>(0.000014)</v>
           </cell>
           <cell r="I27" t="str">
-            <v>0.014</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>DepVarMean</v>
-          </cell>
-          <cell r="B28" t="str">
-            <v>0.070</v>
-          </cell>
-          <cell r="C28" t="str">
-            <v>0.070</v>
-          </cell>
-          <cell r="D28" t="str">
-            <v>0.045</v>
-          </cell>
-          <cell r="E28" t="str">
-            <v>0.045</v>
-          </cell>
-          <cell r="F28" t="str">
-            <v>0.067</v>
-          </cell>
-          <cell r="G28" t="str">
-            <v>0.067</v>
-          </cell>
-          <cell r="H28" t="str">
-            <v>0.047</v>
-          </cell>
-          <cell r="I28" t="str">
-            <v>0.047</v>
+            <v>(0.000014)</v>
           </cell>
         </row>
         <row r="29">
           <cell r="B29" t="str">
-            <v>4667032</v>
+            <v>1298450070</v>
           </cell>
           <cell r="C29" t="str">
-            <v>4667032</v>
+            <v>1298450070</v>
           </cell>
           <cell r="D29" t="str">
-            <v>4629395</v>
+            <v>1287678797</v>
           </cell>
           <cell r="E29" t="str">
-            <v>4629395</v>
+            <v>1287678797</v>
           </cell>
           <cell r="F29" t="str">
-            <v>4667032</v>
+            <v>1298450070</v>
           </cell>
           <cell r="G29" t="str">
-            <v>4667032</v>
+            <v>1298450070</v>
           </cell>
           <cell r="H29" t="str">
-            <v>4629395</v>
+            <v>1287678797</v>
           </cell>
           <cell r="I29" t="str">
-            <v>4629395</v>
+            <v>1287678797</v>
           </cell>
         </row>
       </sheetData>
@@ -1053,7 +1024,7 @@
   <dimension ref="A2:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:L27"/>
+      <selection activeCell="L27" sqref="A3:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1070,54 +1041,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="7"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="11" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="E4" s="6" t="s">
+      <c r="C4" s="11"/>
+      <c r="E4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="H4" s="6" t="s">
+      <c r="F4" s="11"/>
+      <c r="H4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="K4" s="6" t="s">
+      <c r="I4" s="11"/>
+      <c r="K4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="6"/>
+      <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="str">
@@ -1170,19 +1141,19 @@
       </c>
       <c r="C6" s="3" t="str">
         <f>[1]characteristics_switchers!C5</f>
-        <v>-0.011***</v>
+        <v>-0.012***</v>
       </c>
       <c r="E6" s="3" t="str">
         <f>[1]characteristics_switchers!D5</f>
-        <v>-0.0081***</v>
+        <v>-0.0088***</v>
       </c>
       <c r="F6" s="3" t="str">
         <f>[1]characteristics_switchers!E5</f>
-        <v>-0.0076***</v>
+        <v>-0.0078***</v>
       </c>
       <c r="H6" s="3" t="str">
         <f>[1]characteristics_switchers!F5</f>
-        <v>-0.015***</v>
+        <v>-0.016***</v>
       </c>
       <c r="I6" s="3" t="str">
         <f>[1]characteristics_switchers!G5</f>
@@ -1190,11 +1161,11 @@
       </c>
       <c r="K6" s="3" t="str">
         <f>[1]characteristics_switchers!H5</f>
-        <v>-0.0076***</v>
+        <v>-0.0093***</v>
       </c>
       <c r="L6" s="3" t="str">
         <f>[1]characteristics_switchers!I5</f>
-        <v>-0.0069***</v>
+        <v>-0.0086***</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -1208,15 +1179,15 @@
       </c>
       <c r="C7" s="3" t="str">
         <f>[1]characteristics_switchers!C6</f>
-        <v>(0.000016)</v>
+        <v>(0.000017)</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>[1]characteristics_switchers!D6</f>
-        <v>(0.000013)</v>
+        <v>(0.000014)</v>
       </c>
       <c r="F7" s="3" t="str">
         <f>[1]characteristics_switchers!E6</f>
-        <v>(0.000013)</v>
+        <v>(0.000014)</v>
       </c>
       <c r="H7" s="3" t="str">
         <f>[1]characteristics_switchers!F6</f>
@@ -1228,7 +1199,7 @@
       </c>
       <c r="K7" s="3" t="str">
         <f>[1]characteristics_switchers!H6</f>
-        <v>(0.000014)</v>
+        <v>(0.000013)</v>
       </c>
       <c r="L7" s="3" t="str">
         <f>[1]characteristics_switchers!I6</f>
@@ -1241,35 +1212,35 @@
       </c>
       <c r="B8" s="3" t="str">
         <f>[1]characteristics_switchers!B8</f>
-        <v>0.013***</v>
+        <v>0.015***</v>
       </c>
       <c r="C8" s="3" t="str">
         <f>[1]characteristics_switchers!C8</f>
-        <v>0.010***</v>
+        <v>0.012***</v>
       </c>
       <c r="E8" s="3" t="str">
         <f>[1]characteristics_switchers!D8</f>
-        <v>-0.0099***</v>
+        <v>-0.014***</v>
       </c>
       <c r="F8" s="3" t="str">
         <f>[1]characteristics_switchers!E8</f>
-        <v>-0.013***</v>
+        <v>-0.019***</v>
       </c>
       <c r="H8" s="3" t="str">
         <f>[1]characteristics_switchers!F8</f>
-        <v>0.020***</v>
+        <v>0.021***</v>
       </c>
       <c r="I8" s="3" t="str">
         <f>[1]characteristics_switchers!G8</f>
-        <v>0.018***</v>
+        <v>0.019***</v>
       </c>
       <c r="K8" s="3" t="str">
         <f>[1]characteristics_switchers!H8</f>
-        <v>-0.018***</v>
+        <v>-0.0069***</v>
       </c>
       <c r="L8" s="3" t="str">
         <f>[1]characteristics_switchers!I8</f>
-        <v>-0.022***</v>
+        <v>-0.011***</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -1279,27 +1250,27 @@
       </c>
       <c r="B9" s="3" t="str">
         <f>[1]characteristics_switchers!B9</f>
-        <v>(0.000020)</v>
+        <v>(0.000021)</v>
       </c>
       <c r="C9" s="3" t="str">
         <f>[1]characteristics_switchers!C9</f>
-        <v>(0.000020)</v>
+        <v>(0.000022)</v>
       </c>
       <c r="E9" s="3" t="str">
         <f>[1]characteristics_switchers!D9</f>
-        <v>(0.000015)</v>
+        <v>(0.000017)</v>
       </c>
       <c r="F9" s="3" t="str">
         <f>[1]characteristics_switchers!E9</f>
-        <v>(0.000016)</v>
+        <v>(0.000018)</v>
       </c>
       <c r="H9" s="3" t="str">
         <f>[1]characteristics_switchers!F9</f>
-        <v>(0.000019)</v>
+        <v>(0.000021)</v>
       </c>
       <c r="I9" s="3" t="str">
         <f>[1]characteristics_switchers!G9</f>
-        <v>(0.000020)</v>
+        <v>(0.000021)</v>
       </c>
       <c r="K9" s="3" t="str">
         <f>[1]characteristics_switchers!H9</f>
@@ -1324,11 +1295,11 @@
       </c>
       <c r="E10" s="3" t="str">
         <f>[1]characteristics_switchers!D11</f>
-        <v>0.0071***</v>
+        <v>0.010***</v>
       </c>
       <c r="F10" s="3" t="str">
         <f>[1]characteristics_switchers!E11</f>
-        <v>0.0038***</v>
+        <v>0.0060***</v>
       </c>
       <c r="H10" s="3" t="str">
         <f>[1]characteristics_switchers!F11</f>
@@ -1336,15 +1307,15 @@
       </c>
       <c r="I10" s="3" t="str">
         <f>[1]characteristics_switchers!G11</f>
-        <v>0.0086***</v>
+        <v>0.0087***</v>
       </c>
       <c r="K10" s="3" t="str">
         <f>[1]characteristics_switchers!H11</f>
-        <v>0.0099***</v>
+        <v>0.0073***</v>
       </c>
       <c r="L10" s="3" t="str">
         <f>[1]characteristics_switchers!I11</f>
-        <v>0.0058***</v>
+        <v>0.0041***</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -1362,11 +1333,11 @@
       </c>
       <c r="E11" s="3" t="str">
         <f>[1]characteristics_switchers!D12</f>
-        <v>(0.0000086)</v>
+        <v>(0.0000087)</v>
       </c>
       <c r="F11" s="3" t="str">
         <f>[1]characteristics_switchers!E12</f>
-        <v>(0.0000091)</v>
+        <v>(0.0000092)</v>
       </c>
       <c r="H11" s="3" t="str">
         <f>[1]characteristics_switchers!F12</f>
@@ -1378,7 +1349,7 @@
       </c>
       <c r="K11" s="3" t="str">
         <f>[1]characteristics_switchers!H12</f>
-        <v>(0.0000087)</v>
+        <v>(0.0000086)</v>
       </c>
       <c r="L11" s="3" t="str">
         <f>[1]characteristics_switchers!I12</f>
@@ -1391,35 +1362,35 @@
       </c>
       <c r="B12" s="3" t="str">
         <f>[1]characteristics_switchers!B14</f>
-        <v>0.0068***</v>
+        <v>0.0067***</v>
       </c>
       <c r="C12" s="3" t="str">
         <f>[1]characteristics_switchers!C14</f>
-        <v>0.0068***</v>
+        <v>0.0065***</v>
       </c>
       <c r="E12" s="3" t="str">
         <f>[1]characteristics_switchers!D14</f>
-        <v>0.0079***</v>
+        <v>0.0040***</v>
       </c>
       <c r="F12" s="3" t="str">
         <f>[1]characteristics_switchers!E14</f>
-        <v>0.0076***</v>
+        <v>0.0035***</v>
       </c>
       <c r="H12" s="3" t="str">
         <f>[1]characteristics_switchers!F14</f>
-        <v>0.013***</v>
+        <v>0.012***</v>
       </c>
       <c r="I12" s="3" t="str">
         <f>[1]characteristics_switchers!G14</f>
-        <v>0.013***</v>
+        <v>0.012***</v>
       </c>
       <c r="K12" s="3" t="str">
         <f>[1]characteristics_switchers!H14</f>
-        <v>0.0039***</v>
+        <v>0.0076***</v>
       </c>
       <c r="L12" s="3" t="str">
         <f>[1]characteristics_switchers!I14</f>
-        <v>0.0036***</v>
+        <v>0.0072***</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -1429,35 +1400,35 @@
       </c>
       <c r="B13" s="3" t="str">
         <f>[1]characteristics_switchers!B15</f>
-        <v>(0.0000086)</v>
+        <v>(0.0000085)</v>
       </c>
       <c r="C13" s="3" t="str">
         <f>[1]characteristics_switchers!C15</f>
-        <v>(0.0000087)</v>
+        <v>(0.0000086)</v>
       </c>
       <c r="E13" s="3" t="str">
         <f>[1]characteristics_switchers!D15</f>
-        <v>(0.0000066)</v>
+        <v>(0.0000071)</v>
       </c>
       <c r="F13" s="3" t="str">
         <f>[1]characteristics_switchers!E15</f>
-        <v>(0.0000067)</v>
+        <v>(0.0000071)</v>
       </c>
       <c r="H13" s="3" t="str">
         <f>[1]characteristics_switchers!F15</f>
-        <v>(0.0000083)</v>
+        <v>(0.0000082)</v>
       </c>
       <c r="I13" s="3" t="str">
         <f>[1]characteristics_switchers!G15</f>
-        <v>(0.0000084)</v>
+        <v>(0.0000083)</v>
       </c>
       <c r="K13" s="3" t="str">
         <f>[1]characteristics_switchers!H15</f>
-        <v>(0.0000072)</v>
+        <v>(0.0000066)</v>
       </c>
       <c r="L13" s="3" t="str">
         <f>[1]characteristics_switchers!I15</f>
-        <v>(0.0000072)</v>
+        <v>(0.0000067)</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
@@ -1466,35 +1437,35 @@
       </c>
       <c r="B14" s="3" t="str">
         <f>[1]characteristics_switchers!B17</f>
-        <v>-0.0036***</v>
+        <v>0.0035***</v>
       </c>
       <c r="C14" s="3" t="str">
         <f>[1]characteristics_switchers!C17</f>
-        <v>-0.0042***</v>
+        <v>0.0034***</v>
       </c>
       <c r="E14" s="3" t="str">
         <f>[1]characteristics_switchers!D17</f>
-        <v>-0.00036***</v>
+        <v>0.0013***</v>
       </c>
       <c r="F14" s="3" t="str">
         <f>[1]characteristics_switchers!E17</f>
-        <v>-0.00058***</v>
+        <v>0.0013***</v>
       </c>
       <c r="H14" s="3" t="str">
         <f>[1]characteristics_switchers!F17</f>
-        <v>-0.00045***</v>
+        <v>-0.0024***</v>
       </c>
       <c r="I14" s="3" t="str">
         <f>[1]characteristics_switchers!G17</f>
-        <v>-0.00079***</v>
+        <v>-0.0024***</v>
       </c>
       <c r="K14" s="3" t="str">
         <f>[1]characteristics_switchers!H17</f>
-        <v>-0.0011***</v>
+        <v>-0.00060***</v>
       </c>
       <c r="L14" s="3" t="str">
         <f>[1]characteristics_switchers!I17</f>
-        <v>-0.0016***</v>
+        <v>-0.00065***</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -1504,35 +1475,35 @@
       </c>
       <c r="B15" s="3" t="str">
         <f>[1]characteristics_switchers!B18</f>
-        <v>(0.0000050)</v>
+        <v>(0.0000043)</v>
       </c>
       <c r="C15" s="3" t="str">
         <f>[1]characteristics_switchers!C18</f>
-        <v>(0.0000052)</v>
+        <v>(0.0000043)</v>
       </c>
       <c r="E15" s="3" t="str">
         <f>[1]characteristics_switchers!D18</f>
-        <v>(0.0000040)</v>
+        <v>(0.0000035)</v>
       </c>
       <c r="F15" s="3" t="str">
         <f>[1]characteristics_switchers!E18</f>
-        <v>(0.0000041)</v>
+        <v>(0.0000035)</v>
       </c>
       <c r="H15" s="3" t="str">
         <f>[1]characteristics_switchers!F18</f>
-        <v>(0.0000049)</v>
+        <v>(0.0000042)</v>
       </c>
       <c r="I15" s="3" t="str">
         <f>[1]characteristics_switchers!G18</f>
-        <v>(0.0000050)</v>
+        <v>(0.0000042)</v>
       </c>
       <c r="K15" s="3" t="str">
         <f>[1]characteristics_switchers!H18</f>
-        <v>(0.0000042)</v>
+        <v>(0.0000035)</v>
       </c>
       <c r="L15" s="3" t="str">
         <f>[1]characteristics_switchers!I18</f>
-        <v>(0.0000043)</v>
+        <v>(0.0000035)</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
@@ -1545,31 +1516,31 @@
       </c>
       <c r="C16" s="3" t="str">
         <f>[1]characteristics_switchers!C20</f>
-        <v>0.00035***</v>
+        <v>-0.000030</v>
       </c>
       <c r="E16" s="3" t="str">
         <f>[1]characteristics_switchers!D20</f>
-        <v>-0.00045***</v>
+        <v>-0.0060***</v>
       </c>
       <c r="F16" s="3" t="str">
         <f>[1]characteristics_switchers!E20</f>
-        <v>0.0039***</v>
+        <v>-0.0010***</v>
       </c>
       <c r="H16" s="3" t="str">
         <f>[1]characteristics_switchers!F20</f>
-        <v>0.000057**</v>
+        <v>-0.00041***</v>
       </c>
       <c r="I16" s="3" t="str">
         <f>[1]characteristics_switchers!G20</f>
-        <v>0.0034***</v>
+        <v>0.0028***</v>
       </c>
       <c r="K16" s="3" t="str">
         <f>[1]characteristics_switchers!H20</f>
-        <v>-0.0063***</v>
+        <v>-0.00040***</v>
       </c>
       <c r="L16" s="3" t="str">
         <f>[1]characteristics_switchers!I20</f>
-        <v>-0.0011***</v>
+        <v>0.0037***</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
@@ -1587,7 +1558,7 @@
       </c>
       <c r="E17" s="3" t="str">
         <f>[1]characteristics_switchers!D21</f>
-        <v>(0.000021)</v>
+        <v>(0.000020)</v>
       </c>
       <c r="F17" s="3" t="str">
         <f>[1]characteristics_switchers!E21</f>
@@ -1603,7 +1574,7 @@
       </c>
       <c r="K17" s="3" t="str">
         <f>[1]characteristics_switchers!H21</f>
-        <v>(0.000020)</v>
+        <v>(0.000021)</v>
       </c>
       <c r="L17" s="3" t="str">
         <f>[1]characteristics_switchers!I21</f>
@@ -1616,35 +1587,35 @@
       </c>
       <c r="B18" s="3" t="str">
         <f>[1]characteristics_switchers!B23</f>
-        <v>0.00026***</v>
+        <v>-0.0043***</v>
       </c>
       <c r="C18" s="3" t="str">
         <f>[1]characteristics_switchers!C23</f>
-        <v>-0.00022***</v>
+        <v>-0.0032***</v>
       </c>
       <c r="E18" s="3" t="str">
         <f>[1]characteristics_switchers!D23</f>
-        <v>0.0010***</v>
+        <v>-0.0069***</v>
       </c>
       <c r="F18" s="3" t="str">
         <f>[1]characteristics_switchers!E23</f>
-        <v>0.00086***</v>
+        <v>-0.0054***</v>
       </c>
       <c r="H18" s="3" t="str">
         <f>[1]characteristics_switchers!F23</f>
-        <v>0.0013***</v>
+        <v>-0.0033***</v>
       </c>
       <c r="I18" s="3" t="str">
         <f>[1]characteristics_switchers!G23</f>
-        <v>0.0011***</v>
+        <v>-0.0026***</v>
       </c>
       <c r="K18" s="3" t="str">
         <f>[1]characteristics_switchers!H23</f>
-        <v>0.00068***</v>
+        <v>-0.0062***</v>
       </c>
       <c r="L18" s="3" t="str">
         <f>[1]characteristics_switchers!I23</f>
-        <v>0.00033***</v>
+        <v>-0.0049***</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
@@ -1654,35 +1625,35 @@
       </c>
       <c r="B19" s="3" t="str">
         <f>[1]characteristics_switchers!B24</f>
-        <v>(0.000017)</v>
+        <v>(0.000016)</v>
       </c>
       <c r="C19" s="3" t="str">
         <f>[1]characteristics_switchers!C24</f>
-        <v>(0.000018)</v>
+        <v>(0.000016)</v>
       </c>
       <c r="E19" s="3" t="str">
         <f>[1]characteristics_switchers!D24</f>
-        <v>(0.000014)</v>
+        <v>(0.000013)</v>
       </c>
       <c r="F19" s="3" t="str">
         <f>[1]characteristics_switchers!E24</f>
-        <v>(0.000014)</v>
+        <v>(0.000013)</v>
       </c>
       <c r="H19" s="3" t="str">
         <f>[1]characteristics_switchers!F24</f>
-        <v>(0.000017)</v>
+        <v>(0.000016)</v>
       </c>
       <c r="I19" s="3" t="str">
         <f>[1]characteristics_switchers!G24</f>
-        <v>(0.000018)</v>
+        <v>(0.000016)</v>
       </c>
       <c r="K19" s="3" t="str">
         <f>[1]characteristics_switchers!H24</f>
-        <v>(0.000014)</v>
+        <v>(0.000013)</v>
       </c>
       <c r="L19" s="3" t="str">
         <f>[1]characteristics_switchers!I24</f>
-        <v>(0.000015)</v>
+        <v>(0.000013)</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
@@ -1691,38 +1662,38 @@
       </c>
       <c r="B21" s="4" t="str">
         <f>[1]characteristics_switchers!B29</f>
-        <v>4667032</v>
+        <v>1298450070</v>
       </c>
       <c r="C21" s="4" t="str">
         <f>[1]characteristics_switchers!C29</f>
-        <v>4667032</v>
+        <v>1298450070</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="str">
         <f>[1]characteristics_switchers!D29</f>
-        <v>4629395</v>
+        <v>1287678797</v>
       </c>
       <c r="F21" s="4" t="str">
         <f>[1]characteristics_switchers!E29</f>
-        <v>4629395</v>
+        <v>1287678797</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4" t="str">
         <f>[1]characteristics_switchers!F29</f>
-        <v>4667032</v>
+        <v>1298450070</v>
       </c>
       <c r="I21" s="4" t="str">
         <f>[1]characteristics_switchers!G29</f>
-        <v>4667032</v>
+        <v>1298450070</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4" t="str">
         <f>[1]characteristics_switchers!H29</f>
-        <v>4629395</v>
+        <v>1287678797</v>
       </c>
       <c r="L21" s="4" t="str">
         <f>[1]characteristics_switchers!I29</f>
-        <v>4629395</v>
+        <v>1287678797</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
@@ -1731,111 +1702,73 @@
       </c>
       <c r="B22" s="3" t="str">
         <f>[1]characteristics_switchers!B26</f>
-        <v>1298450070</v>
+        <v>0.00022***</v>
       </c>
       <c r="C22" s="3" t="str">
         <f>[1]characteristics_switchers!C26</f>
-        <v>1298450070</v>
+        <v>-0.00023***</v>
       </c>
       <c r="E22" s="3" t="str">
         <f>[1]characteristics_switchers!D26</f>
-        <v>1287678797</v>
+        <v>0.00069***</v>
       </c>
       <c r="F22" s="3" t="str">
         <f>[1]characteristics_switchers!E26</f>
-        <v>1287678797</v>
+        <v>0.00034***</v>
       </c>
       <c r="H22" s="3" t="str">
         <f>[1]characteristics_switchers!F26</f>
-        <v>1298450070</v>
+        <v>0.0013***</v>
       </c>
       <c r="I22" s="3" t="str">
         <f>[1]characteristics_switchers!G26</f>
-        <v>1298450070</v>
+        <v>0.0011***</v>
       </c>
       <c r="K22" s="3" t="str">
         <f>[1]characteristics_switchers!H26</f>
-        <v>1287678797</v>
+        <v>0.0010***</v>
       </c>
       <c r="L22" s="3" t="str">
         <f>[1]characteristics_switchers!I26</f>
-        <v>1287678797</v>
+        <v>0.00088***</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f>[1]characteristics_switchers!A27</f>
-        <v>R-sq</v>
+        <v/>
       </c>
       <c r="B23" s="3" t="str">
         <f>[1]characteristics_switchers!B27</f>
-        <v>0.009</v>
+        <v>(0.000017)</v>
       </c>
       <c r="C23" s="3" t="str">
         <f>[1]characteristics_switchers!C27</f>
-        <v>0.013</v>
+        <v>(0.000018)</v>
       </c>
       <c r="E23" s="3" t="str">
         <f>[1]characteristics_switchers!D27</f>
-        <v>0.012</v>
+        <v>(0.000014)</v>
       </c>
       <c r="F23" s="3" t="str">
         <f>[1]characteristics_switchers!E27</f>
-        <v>0.016</v>
+        <v>(0.000015)</v>
       </c>
       <c r="H23" s="3" t="str">
         <f>[1]characteristics_switchers!F27</f>
-        <v>0.008</v>
+        <v>(0.000017)</v>
       </c>
       <c r="I23" s="3" t="str">
         <f>[1]characteristics_switchers!G27</f>
-        <v>0.011</v>
+        <v>(0.000018)</v>
       </c>
       <c r="K23" s="3" t="str">
         <f>[1]characteristics_switchers!H27</f>
-        <v>0.009</v>
+        <v>(0.000014)</v>
       </c>
       <c r="L23" s="3" t="str">
         <f>[1]characteristics_switchers!I27</f>
-        <v>0.014</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" t="str">
-        <f>[1]characteristics_switchers!A28</f>
-        <v>DepVarMean</v>
-      </c>
-      <c r="B24" s="3" t="str">
-        <f>[1]characteristics_switchers!B28</f>
-        <v>0.070</v>
-      </c>
-      <c r="C24" s="3" t="str">
-        <f>[1]characteristics_switchers!C28</f>
-        <v>0.070</v>
-      </c>
-      <c r="E24" s="3" t="str">
-        <f>[1]characteristics_switchers!D28</f>
-        <v>0.045</v>
-      </c>
-      <c r="F24" s="3" t="str">
-        <f>[1]characteristics_switchers!E28</f>
-        <v>0.045</v>
-      </c>
-      <c r="H24" s="3" t="str">
-        <f>[1]characteristics_switchers!F28</f>
-        <v>0.067</v>
-      </c>
-      <c r="I24" s="3" t="str">
-        <f>[1]characteristics_switchers!G28</f>
-        <v>0.067</v>
-      </c>
-      <c r="K24" s="3" t="str">
-        <f>[1]characteristics_switchers!H28</f>
-        <v>0.047</v>
-      </c>
-      <c r="L24" s="3" t="str">
-        <f>[1]characteristics_switchers!I28</f>
-        <v>0.047</v>
+        <v>(0.000014)</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>